<commit_message>
Host a web application with Azure App Service
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51219611-5270-468F-85F7-1E8AF8AD66F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E82F1CC-619B-4586-AA45-FB805B149A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="133">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -429,13 +429,19 @@
   </si>
   <si>
     <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/DGQWWE3J?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/N794SLSF?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Control%20Azure%20services%20with%20the%20CLI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1010,11 +1016,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50.33203125" customWidth="1"/>
     <col min="2" max="2" width="103.88671875" customWidth="1"/>
@@ -1024,7 +1030,7 @@
     <col min="7" max="7" width="152.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.4" customHeight="1">
+    <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>97</v>
       </c>
@@ -1032,7 +1038,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24.6" customHeight="1">
+    <row r="2" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="14" t="s">
         <v>73</v>
       </c>
@@ -1055,7 +1061,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
         <v>74</v>
       </c>
@@ -1078,7 +1084,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="23"/>
       <c r="B4" s="12" t="s">
         <v>2</v>
@@ -1096,7 +1102,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.4" customHeight="1">
+    <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="23"/>
       <c r="B5" s="12" t="s">
         <v>3</v>
@@ -1114,7 +1120,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -1123,7 +1129,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="23"/>
       <c r="B7" s="13" t="s">
         <v>5</v>
@@ -1141,7 +1147,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="23"/>
       <c r="B8" s="10" t="s">
         <v>6</v>
@@ -1162,7 +1168,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="23"/>
       <c r="B9" s="12" t="s">
         <v>7</v>
@@ -1180,7 +1186,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="23"/>
       <c r="B10" s="12" t="s">
         <v>8</v>
@@ -1198,7 +1204,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="12" t="s">
         <v>9</v>
@@ -1216,7 +1222,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="23"/>
       <c r="B12" s="12" t="s">
         <v>10</v>
@@ -1234,7 +1240,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="23"/>
       <c r="B13" s="12" t="s">
         <v>11</v>
@@ -1252,7 +1258,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="23"/>
       <c r="B14" s="18" t="s">
         <v>12</v>
@@ -1261,16 +1267,28 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="23"/>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="C15" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="6">
+        <v>45339</v>
+      </c>
+      <c r="E15" s="6">
+        <v>45339</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="23"/>
       <c r="B16" s="4" t="s">
         <v>14</v>
@@ -1279,7 +1297,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="23"/>
       <c r="B17" s="10" t="s">
         <v>15</v>
@@ -1300,7 +1318,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="23"/>
       <c r="B18" s="10" t="s">
         <v>16</v>
@@ -1321,7 +1339,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="23"/>
       <c r="B19" s="2" t="s">
         <v>17</v>
@@ -1330,7 +1348,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="23"/>
       <c r="B20" s="10" t="s">
         <v>18</v>
@@ -1351,7 +1369,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="23"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
@@ -1360,7 +1378,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="23"/>
       <c r="B22" s="2" t="s">
         <v>20</v>
@@ -1369,7 +1387,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="23"/>
       <c r="B23" s="2" t="s">
         <v>21</v>
@@ -1378,7 +1396,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
       <c r="B24" s="2" t="s">
         <v>22</v>
@@ -1387,7 +1405,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="23"/>
       <c r="B25" s="2" t="s">
         <v>23</v>
@@ -1396,7 +1414,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="23"/>
       <c r="B26" s="12" t="s">
         <v>24</v>
@@ -1414,7 +1432,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="23"/>
       <c r="B27" s="2" t="s">
         <v>25</v>
@@ -1423,7 +1441,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="23"/>
       <c r="B28" s="10" t="s">
         <v>26</v>
@@ -1444,7 +1462,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="23"/>
       <c r="B29" s="10" t="s">
         <v>27</v>
@@ -1465,7 +1483,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="23"/>
       <c r="B30" s="2" t="s">
         <v>28</v>
@@ -1474,7 +1492,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="23"/>
       <c r="B31" s="10" t="s">
         <v>29</v>
@@ -1492,7 +1510,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="23"/>
       <c r="B32" s="2" t="s">
         <v>30</v>
@@ -1501,7 +1519,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="23"/>
       <c r="B33" s="2" t="s">
         <v>31</v>
@@ -1510,7 +1528,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="23"/>
       <c r="B34" s="2" t="s">
         <v>32</v>
@@ -1519,7 +1537,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="23"/>
       <c r="B35" s="2" t="s">
         <v>33</v>
@@ -1528,7 +1546,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="23"/>
       <c r="B36" s="12" t="s">
         <v>34</v>
@@ -1546,7 +1564,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="23"/>
       <c r="B37" s="2" t="s">
         <v>35</v>
@@ -1555,7 +1573,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="23"/>
       <c r="B38" s="2" t="s">
         <v>36</v>
@@ -1564,7 +1582,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="23"/>
       <c r="B39" s="2" t="s">
         <v>37</v>
@@ -1573,7 +1591,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="23"/>
       <c r="B40" s="2" t="s">
         <v>38</v>
@@ -1582,7 +1600,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="23"/>
       <c r="B41" s="2" t="s">
         <v>39</v>
@@ -1591,7 +1609,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="23"/>
       <c r="B42" s="2" t="s">
         <v>40</v>
@@ -1600,7 +1618,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="23"/>
       <c r="B43" s="2" t="s">
         <v>41</v>
@@ -1609,7 +1627,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="23"/>
       <c r="B44" s="2" t="s">
         <v>42</v>
@@ -1618,7 +1636,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="23"/>
       <c r="B45" s="2" t="s">
         <v>43</v>
@@ -1627,7 +1645,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="23"/>
       <c r="B46" s="2" t="s">
         <v>44</v>
@@ -1636,7 +1654,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="23"/>
       <c r="B47" s="2" t="s">
         <v>45</v>
@@ -1645,7 +1663,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="23"/>
       <c r="B48" s="2" t="s">
         <v>46</v>
@@ -1654,7 +1672,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="23"/>
       <c r="B49" s="2" t="s">
         <v>47</v>
@@ -1663,7 +1681,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="23"/>
       <c r="B50" s="22" t="s">
         <v>48</v>
@@ -1672,7 +1690,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="23"/>
       <c r="B51" s="2" t="s">
         <v>49</v>
@@ -1681,7 +1699,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="23"/>
       <c r="B52" s="2" t="s">
         <v>50</v>
@@ -1690,7 +1708,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="23"/>
       <c r="B53" s="2" t="s">
         <v>51</v>
@@ -1699,7 +1717,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="23"/>
       <c r="B54" s="2" t="s">
         <v>52</v>
@@ -1708,7 +1726,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="23"/>
       <c r="B55" s="2" t="s">
         <v>53</v>
@@ -1717,7 +1735,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="23"/>
       <c r="B56" s="2" t="s">
         <v>54</v>
@@ -1726,7 +1744,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="23"/>
       <c r="B57" s="2" t="s">
         <v>55</v>
@@ -1735,7 +1753,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="23"/>
       <c r="B58" s="2" t="s">
         <v>56</v>
@@ -1744,7 +1762,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="23"/>
       <c r="B59" s="10" t="s">
         <v>57</v>
@@ -1765,7 +1783,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="23"/>
       <c r="B60" s="10" t="s">
         <v>58</v>
@@ -1783,7 +1801,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="23"/>
       <c r="B61" s="11" t="s">
         <v>59</v>
@@ -1804,7 +1822,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="23"/>
       <c r="B62" s="10" t="s">
         <v>60</v>
@@ -1825,7 +1843,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="23"/>
       <c r="B63" s="2" t="s">
         <v>61</v>
@@ -1834,7 +1852,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="23"/>
       <c r="B64" s="2" t="s">
         <v>62</v>
@@ -1843,7 +1861,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="23"/>
       <c r="B65" s="10" t="s">
         <v>63</v>
@@ -1864,7 +1882,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="23"/>
       <c r="B66" s="2" t="s">
         <v>64</v>
@@ -1873,7 +1891,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="23"/>
       <c r="B67" t="s">
         <v>65</v>
@@ -1882,7 +1900,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="23"/>
       <c r="B68" s="10" t="s">
         <v>66</v>
@@ -1903,7 +1921,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="23"/>
       <c r="B69" t="s">
         <v>67</v>
@@ -1912,7 +1930,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="23"/>
       <c r="B70" s="2" t="s">
         <v>68</v>
@@ -1921,7 +1939,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="23"/>
       <c r="B71" t="s">
         <v>69</v>
@@ -1930,7 +1948,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="23"/>
       <c r="B72" s="18" t="s">
         <v>70</v>
@@ -1939,71 +1957,71 @@
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="2:2">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="2:2">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="2:2">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="2:2">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="2:2">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="2:2">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="2:2">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="2:2">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="2:2">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="2:2">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="2:2">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="92" spans="2:2">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="93" spans="2:2">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="94" spans="2:2">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="2" t="s">
         <v>75</v>
       </c>
@@ -2050,9 +2068,11 @@
     <hyperlink ref="G62" r:id="rId35" xr:uid="{3498D723-71A2-4C81-9ABA-DE730BCFB2FD}"/>
     <hyperlink ref="G65" r:id="rId36" xr:uid="{3196769D-227A-45EA-8497-C658DDBB6FDF}"/>
     <hyperlink ref="G68" r:id="rId37" xr:uid="{8530BA66-C1DD-4A6B-B09C-354C65A59BC7}"/>
+    <hyperlink ref="G15" r:id="rId38" xr:uid="{EF41FD36-48D6-4F77-A3DC-D3B1A59E63E4}"/>
+    <hyperlink ref="F15" r:id="rId39" xr:uid="{FFF7918C-C271-4715-8A9E-33714A21A205}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId38"/>
+  <pageSetup orientation="portrait" r:id="rId40"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Review the principles of code debugging and exception handling
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E82F1CC-619B-4586-AA45-FB805B149A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEA63FA-0EFE-4EAF-BF14-0D1B695D97CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="135">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -435,13 +435,19 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Control%20Azure%20services%20with%20the%20CLI</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/HYGQ56A8?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Host%20a%20web%20application%20with%20Azure%20App%20Service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -651,7 +657,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -679,6 +684,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1016,11 +1022,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="50.33203125" customWidth="1"/>
     <col min="2" max="2" width="103.88671875" customWidth="1"/>
@@ -1030,998 +1036,1010 @@
     <col min="7" max="7" width="152.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:7" ht="26.4" customHeight="1">
+      <c r="A1" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="14" t="s">
+    <row r="2" spans="1:7" ht="24.6" customHeight="1">
+      <c r="A2" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="14" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:7">
+      <c r="A3" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D3" s="6">
+      <c r="C3" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="5">
         <v>45325</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>45325</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="23"/>
-      <c r="B4" s="12" t="s">
+    <row r="4" spans="1:7">
+      <c r="A4" s="22"/>
+      <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="6">
+      <c r="C4" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="5">
         <v>45338</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>45338</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="23"/>
-      <c r="B5" s="12" t="s">
+    <row r="5" spans="1:7" ht="14.4" customHeight="1">
+      <c r="A5" s="22"/>
+      <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="C5" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D5" s="5">
         <v>45338</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>45338</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="23"/>
+    <row r="6" spans="1:7">
+      <c r="A6" s="22"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="13" t="s">
+      <c r="C6" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="22"/>
+      <c r="B7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="6">
+      <c r="C7" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="5">
         <v>45338</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>45338</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="6" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="23"/>
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:7">
+      <c r="A8" s="22"/>
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="6">
+      <c r="C8" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D8" s="5">
         <v>45237</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>45237</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G8" s="7" t="s">
+      <c r="G8" s="6" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="23"/>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:7">
+      <c r="A9" s="22"/>
+      <c r="B9" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D9" s="6">
+      <c r="C9" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D9" s="5">
         <v>45334</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>45334</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="6" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="23"/>
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:7">
+      <c r="A10" s="22"/>
+      <c r="B10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="6">
+      <c r="C10" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" s="5">
         <v>45338</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>45338</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="23"/>
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="1:7">
+      <c r="A11" s="22"/>
+      <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="6">
+      <c r="C11" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" s="5">
         <v>45337</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>45337</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="23"/>
-      <c r="B12" s="12" t="s">
+    <row r="12" spans="1:7">
+      <c r="A12" s="22"/>
+      <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="6">
+      <c r="C12" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D12" s="5">
         <v>45338</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>45338</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="6" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="23"/>
-      <c r="B13" s="12" t="s">
+    <row r="13" spans="1:7">
+      <c r="A13" s="22"/>
+      <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="C13" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="5">
         <v>45338</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>45338</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="23"/>
-      <c r="B14" s="18" t="s">
+    <row r="14" spans="1:7">
+      <c r="A14" s="22"/>
+      <c r="B14" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="23"/>
-      <c r="B15" s="10" t="s">
+    <row r="15" spans="1:7">
+      <c r="A15" s="22"/>
+      <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="6">
+      <c r="C15" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="5">
         <v>45339</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="5">
         <v>45339</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="G15" s="6" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="23"/>
-      <c r="B16" s="4" t="s">
+    <row r="16" spans="1:7">
+      <c r="A16" s="22"/>
+      <c r="B16" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="23"/>
-      <c r="B17" s="10" t="s">
+      <c r="C16" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="5">
+        <v>45339</v>
+      </c>
+      <c r="E16" s="5">
+        <v>45339</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="22"/>
+      <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D17" s="6">
+      <c r="C17" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="5">
         <v>45335</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="5">
         <v>45335</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="7" t="s">
+      <c r="G17" s="6" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="23"/>
-      <c r="B18" s="10" t="s">
+    <row r="18" spans="1:7">
+      <c r="A18" s="22"/>
+      <c r="B18" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D18" s="6">
+      <c r="C18" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="5">
         <v>45335</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="5">
         <v>45335</v>
       </c>
-      <c r="F18" s="7" t="s">
+      <c r="F18" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="G18" s="7" t="s">
+      <c r="G18" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="23"/>
+    <row r="19" spans="1:7">
+      <c r="A19" s="22"/>
       <c r="B19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="23"/>
-      <c r="B20" s="10" t="s">
+      <c r="C19" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="22"/>
+      <c r="B20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D20" s="6">
+      <c r="C20" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="5">
         <v>45337</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="5">
         <v>45337</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="23"/>
+    <row r="21" spans="1:7">
+      <c r="A21" s="22"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="23"/>
+      <c r="C21" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="22"/>
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="23"/>
+      <c r="C22" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="22"/>
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="23"/>
+      <c r="C23" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="22"/>
       <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="23"/>
+      <c r="C24" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="22"/>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="23"/>
-      <c r="B26" s="12" t="s">
+      <c r="C25" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="22"/>
+      <c r="B26" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="6">
+      <c r="C26" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D26" s="5">
         <v>45338</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="5">
         <v>45339</v>
       </c>
-      <c r="F26" s="7" t="s">
+      <c r="F26" s="6" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="23"/>
+    <row r="27" spans="1:7">
+      <c r="A27" s="22"/>
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="23"/>
-      <c r="B28" s="10" t="s">
+      <c r="C27" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="22"/>
+      <c r="B28" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" s="6">
+      <c r="C28" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D28" s="5">
         <v>45335</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="5">
         <v>45335</v>
       </c>
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="G28" s="7" t="s">
+      <c r="G28" s="6" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="23"/>
-      <c r="B29" s="10" t="s">
+    <row r="29" spans="1:7">
+      <c r="A29" s="22"/>
+      <c r="B29" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D29" s="6">
+      <c r="C29" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="5">
         <v>45337</v>
       </c>
-      <c r="E29" s="6">
+      <c r="E29" s="5">
         <v>45337</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="G29" s="7" t="s">
+      <c r="G29" s="6" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="23"/>
+    <row r="30" spans="1:7">
+      <c r="A30" s="22"/>
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="23"/>
-      <c r="B31" s="10" t="s">
+      <c r="C30" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="22"/>
+      <c r="B31" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" s="6">
+      <c r="C31" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D31" s="5">
         <v>45337</v>
       </c>
-      <c r="E31" s="6">
+      <c r="E31" s="5">
         <v>45337</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="6" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="23"/>
+    <row r="32" spans="1:7">
+      <c r="A32" s="22"/>
       <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="23"/>
+      <c r="C32" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="22"/>
       <c r="B33" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="23"/>
+      <c r="C33" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="22"/>
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="23"/>
+      <c r="C34" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="22"/>
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="23"/>
-      <c r="B36" s="12" t="s">
+      <c r="C35" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="22"/>
+      <c r="B36" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D36" s="6">
+      <c r="C36" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="5">
         <v>45337</v>
       </c>
-      <c r="E36" s="6">
+      <c r="E36" s="5">
         <v>45337</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="23"/>
+    <row r="37" spans="1:6">
+      <c r="A37" s="22"/>
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="23"/>
+      <c r="C37" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="22"/>
       <c r="B38" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="23"/>
+      <c r="C38" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="22"/>
       <c r="B39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="23"/>
+      <c r="C39" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="22"/>
       <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="23"/>
+      <c r="C40" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="22"/>
       <c r="B41" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="23"/>
+      <c r="C41" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="22"/>
       <c r="B42" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="23"/>
+      <c r="C42" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="22"/>
       <c r="B43" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C43" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="23"/>
+      <c r="C43" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="22"/>
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="23"/>
+      <c r="C44" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="22"/>
       <c r="B45" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C45" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="23"/>
+      <c r="C45" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="22"/>
       <c r="B46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="23"/>
+      <c r="C46" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="22"/>
       <c r="B47" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="23"/>
+      <c r="C47" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="22"/>
       <c r="B48" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="23"/>
+      <c r="C48" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="22"/>
       <c r="B49" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C49" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="23"/>
-      <c r="B50" s="22" t="s">
+      <c r="C49" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="22"/>
+      <c r="B50" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="20" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="23"/>
+    <row r="51" spans="1:7">
+      <c r="A51" s="22"/>
       <c r="B51" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="23"/>
+      <c r="C51" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="22"/>
       <c r="B52" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="23"/>
+      <c r="C52" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="22"/>
       <c r="B53" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C53" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="23"/>
+      <c r="C53" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="22"/>
       <c r="B54" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="23"/>
+      <c r="C54" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="22"/>
       <c r="B55" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="23"/>
+      <c r="C55" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="22"/>
       <c r="B56" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C56" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="23"/>
+      <c r="C56" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
+      <c r="A57" s="22"/>
       <c r="B57" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C57" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="23"/>
+      <c r="C57" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="22"/>
       <c r="B58" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="23"/>
-      <c r="B59" s="10" t="s">
+      <c r="C58" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="22"/>
+      <c r="B59" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C59" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D59" s="6">
+      <c r="C59" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D59" s="5">
         <v>45336</v>
       </c>
-      <c r="E59" s="6">
+      <c r="E59" s="5">
         <v>45336</v>
       </c>
-      <c r="F59" s="7" t="s">
+      <c r="F59" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G59" s="7" t="s">
+      <c r="G59" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="23"/>
-      <c r="B60" s="10" t="s">
+    <row r="60" spans="1:7">
+      <c r="A60" s="22"/>
+      <c r="B60" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C60" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D60" s="6">
+      <c r="C60" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="5">
         <v>45337</v>
       </c>
-      <c r="E60" s="6">
+      <c r="E60" s="5">
         <v>45337</v>
       </c>
-      <c r="F60" s="7" t="s">
+      <c r="F60" s="6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="23"/>
-      <c r="B61" s="11" t="s">
+    <row r="61" spans="1:7">
+      <c r="A61" s="22"/>
+      <c r="B61" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="C61" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D61" s="6">
+      <c r="C61" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D61" s="5">
         <v>45336</v>
       </c>
-      <c r="E61" s="6">
+      <c r="E61" s="5">
         <v>45336</v>
       </c>
-      <c r="F61" s="7" t="s">
+      <c r="F61" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="G61" s="7" t="s">
+      <c r="G61" s="6" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="23"/>
-      <c r="B62" s="10" t="s">
+    <row r="62" spans="1:7">
+      <c r="A62" s="22"/>
+      <c r="B62" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C62" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D62" s="6">
+      <c r="C62" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D62" s="5">
         <v>45337</v>
       </c>
-      <c r="E62" s="6">
+      <c r="E62" s="5">
         <v>45337</v>
       </c>
-      <c r="F62" s="7" t="s">
+      <c r="F62" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G62" s="7" t="s">
+      <c r="G62" s="6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="23"/>
+    <row r="63" spans="1:7">
+      <c r="A63" s="22"/>
       <c r="B63" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C63" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="23"/>
+      <c r="C63" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
+      <c r="A64" s="22"/>
       <c r="B64" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C64" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="23"/>
-      <c r="B65" s="10" t="s">
+      <c r="C64" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
+      <c r="A65" s="22"/>
+      <c r="B65" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C65" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D65" s="6">
+      <c r="C65" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D65" s="5">
         <v>45337</v>
       </c>
-      <c r="E65" s="6">
+      <c r="E65" s="5">
         <v>45337</v>
       </c>
-      <c r="F65" s="7" t="s">
+      <c r="F65" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G65" s="7" t="s">
+      <c r="G65" s="6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="23"/>
+    <row r="66" spans="1:7">
+      <c r="A66" s="22"/>
       <c r="B66" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C66" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="23"/>
+      <c r="C66" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
+      <c r="A67" s="22"/>
       <c r="B67" t="s">
         <v>65</v>
       </c>
-      <c r="C67" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="23"/>
-      <c r="B68" s="10" t="s">
+      <c r="C67" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
+      <c r="A68" s="22"/>
+      <c r="B68" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C68" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="D68" s="6">
+      <c r="C68" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D68" s="5">
         <v>45336</v>
       </c>
-      <c r="E68" s="6">
+      <c r="E68" s="5">
         <v>45336</v>
       </c>
-      <c r="F68" s="7" t="s">
+      <c r="F68" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G68" s="7" t="s">
+      <c r="G68" s="6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="23"/>
+    <row r="69" spans="1:7">
+      <c r="A69" s="22"/>
       <c r="B69" t="s">
         <v>67</v>
       </c>
-      <c r="C69" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="23"/>
+      <c r="C69" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70" s="22"/>
       <c r="B70" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C70" s="17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="23"/>
+      <c r="C70" s="16" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71" s="22"/>
       <c r="B71" t="s">
         <v>69</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="19" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="23"/>
-      <c r="B72" s="18" t="s">
+    <row r="72" spans="1:7">
+      <c r="A72" s="22"/>
+      <c r="B72" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C72" s="19" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7">
       <c r="B80" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:2">
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:2">
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:2">
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:2">
       <c r="B84" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:2">
       <c r="B85" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:2">
       <c r="B86" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:2">
       <c r="B87" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:2">
       <c r="B88" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:2">
       <c r="B89" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:2">
       <c r="B90" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:2">
       <c r="B91" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:2">
       <c r="B92" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B93" s="5" t="s">
+    <row r="93" spans="2:2">
+      <c r="B93" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:2">
       <c r="B94" s="2" t="s">
         <v>75</v>
       </c>
@@ -2070,9 +2088,11 @@
     <hyperlink ref="G68" r:id="rId37" xr:uid="{8530BA66-C1DD-4A6B-B09C-354C65A59BC7}"/>
     <hyperlink ref="G15" r:id="rId38" xr:uid="{EF41FD36-48D6-4F77-A3DC-D3B1A59E63E4}"/>
     <hyperlink ref="F15" r:id="rId39" xr:uid="{FFF7918C-C271-4715-8A9E-33714A21A205}"/>
+    <hyperlink ref="G16" r:id="rId40" xr:uid="{9EF2E5E4-26B3-4594-BB2E-BBAA5C4C11DB}"/>
+    <hyperlink ref="F16" r:id="rId41" xr:uid="{0DE4CF76-CC43-4FEB-B7C5-C32B4DA42AC2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId40"/>
+  <pageSetup orientation="portrait" r:id="rId42"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Choose a data storage approach in Azure
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEA63FA-0EFE-4EAF-BF14-0D1B695D97CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1448C624-0138-4FE6-B636-0DCFA4E28685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="137">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -441,13 +441,19 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Host%20a%20web%20application%20with%20Azure%20App%20Service</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/8R6ECDVW?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Review%20the%20principles%20of%20code%20debugging%20and%20exception%20handling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1022,11 +1028,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50.33203125" customWidth="1"/>
     <col min="2" max="2" width="103.88671875" customWidth="1"/>
@@ -1036,7 +1042,7 @@
     <col min="7" max="7" width="152.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26.4" customHeight="1">
+    <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>97</v>
       </c>
@@ -1044,7 +1050,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24.6" customHeight="1">
+    <row r="2" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="13" t="s">
         <v>73</v>
       </c>
@@ -1067,7 +1073,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="22" t="s">
         <v>74</v>
       </c>
@@ -1090,7 +1096,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="22"/>
       <c r="B4" s="11" t="s">
         <v>2</v>
@@ -1108,7 +1114,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.4" customHeight="1">
+    <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="22"/>
       <c r="B5" s="11" t="s">
         <v>3</v>
@@ -1126,7 +1132,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="22"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -1135,7 +1141,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="22"/>
       <c r="B7" s="12" t="s">
         <v>5</v>
@@ -1153,7 +1159,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="22"/>
       <c r="B8" s="9" t="s">
         <v>6</v>
@@ -1174,7 +1180,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="22"/>
       <c r="B9" s="11" t="s">
         <v>7</v>
@@ -1192,7 +1198,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="22"/>
       <c r="B10" s="11" t="s">
         <v>8</v>
@@ -1210,7 +1216,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="22"/>
       <c r="B11" s="11" t="s">
         <v>9</v>
@@ -1228,7 +1234,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="22"/>
       <c r="B12" s="11" t="s">
         <v>10</v>
@@ -1246,7 +1252,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="22"/>
       <c r="B13" s="11" t="s">
         <v>11</v>
@@ -1264,7 +1270,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="22"/>
       <c r="B14" s="17" t="s">
         <v>12</v>
@@ -1273,7 +1279,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="22"/>
       <c r="B15" s="9" t="s">
         <v>13</v>
@@ -1294,7 +1300,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="22"/>
       <c r="B16" s="23" t="s">
         <v>14</v>
@@ -1315,7 +1321,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="22"/>
       <c r="B17" s="9" t="s">
         <v>15</v>
@@ -1336,7 +1342,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="22"/>
       <c r="B18" s="9" t="s">
         <v>16</v>
@@ -1357,16 +1363,28 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="22"/>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="C19" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="5">
+        <v>45339</v>
+      </c>
+      <c r="E19" s="5">
+        <v>45339</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="22"/>
       <c r="B20" s="9" t="s">
         <v>18</v>
@@ -1387,7 +1405,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
       <c r="B21" s="2" t="s">
         <v>19</v>
@@ -1396,7 +1414,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="22"/>
       <c r="B22" s="2" t="s">
         <v>20</v>
@@ -1405,7 +1423,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="2" t="s">
         <v>21</v>
@@ -1414,7 +1432,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="22"/>
       <c r="B24" s="2" t="s">
         <v>22</v>
@@ -1423,7 +1441,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="22"/>
       <c r="B25" s="2" t="s">
         <v>23</v>
@@ -1432,7 +1450,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="22"/>
       <c r="B26" s="11" t="s">
         <v>24</v>
@@ -1450,7 +1468,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="22"/>
       <c r="B27" s="2" t="s">
         <v>25</v>
@@ -1459,7 +1477,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="22"/>
       <c r="B28" s="9" t="s">
         <v>26</v>
@@ -1480,7 +1498,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="22"/>
       <c r="B29" s="9" t="s">
         <v>27</v>
@@ -1501,7 +1519,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="22"/>
       <c r="B30" s="2" t="s">
         <v>28</v>
@@ -1510,7 +1528,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="22"/>
       <c r="B31" s="9" t="s">
         <v>29</v>
@@ -1528,7 +1546,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="22"/>
       <c r="B32" s="2" t="s">
         <v>30</v>
@@ -1537,7 +1555,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="22"/>
       <c r="B33" s="2" t="s">
         <v>31</v>
@@ -1546,7 +1564,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="22"/>
       <c r="B34" s="2" t="s">
         <v>32</v>
@@ -1555,7 +1573,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="22"/>
       <c r="B35" s="2" t="s">
         <v>33</v>
@@ -1564,7 +1582,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="22"/>
       <c r="B36" s="11" t="s">
         <v>34</v>
@@ -1582,7 +1600,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="22"/>
       <c r="B37" s="2" t="s">
         <v>35</v>
@@ -1591,7 +1609,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="22"/>
       <c r="B38" s="2" t="s">
         <v>36</v>
@@ -1600,7 +1618,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="22"/>
       <c r="B39" s="2" t="s">
         <v>37</v>
@@ -1609,7 +1627,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="22"/>
       <c r="B40" s="2" t="s">
         <v>38</v>
@@ -1618,7 +1636,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="22"/>
       <c r="B41" s="2" t="s">
         <v>39</v>
@@ -1627,7 +1645,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="22"/>
       <c r="B42" s="2" t="s">
         <v>40</v>
@@ -1636,7 +1654,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="22"/>
       <c r="B43" s="2" t="s">
         <v>41</v>
@@ -1645,7 +1663,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="22"/>
       <c r="B44" s="2" t="s">
         <v>42</v>
@@ -1654,7 +1672,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="22"/>
       <c r="B45" s="2" t="s">
         <v>43</v>
@@ -1663,7 +1681,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="22"/>
       <c r="B46" s="2" t="s">
         <v>44</v>
@@ -1672,7 +1690,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="22"/>
       <c r="B47" s="2" t="s">
         <v>45</v>
@@ -1681,7 +1699,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="22"/>
       <c r="B48" s="2" t="s">
         <v>46</v>
@@ -1690,7 +1708,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="22"/>
       <c r="B49" s="2" t="s">
         <v>47</v>
@@ -1699,7 +1717,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="22"/>
       <c r="B50" s="21" t="s">
         <v>48</v>
@@ -1708,7 +1726,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="22"/>
       <c r="B51" s="2" t="s">
         <v>49</v>
@@ -1717,7 +1735,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="22"/>
       <c r="B52" s="2" t="s">
         <v>50</v>
@@ -1726,7 +1744,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="22"/>
       <c r="B53" s="2" t="s">
         <v>51</v>
@@ -1735,7 +1753,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="22"/>
       <c r="B54" s="2" t="s">
         <v>52</v>
@@ -1744,7 +1762,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="22"/>
       <c r="B55" s="2" t="s">
         <v>53</v>
@@ -1753,7 +1771,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="22"/>
       <c r="B56" s="2" t="s">
         <v>54</v>
@@ -1762,7 +1780,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="22"/>
       <c r="B57" s="2" t="s">
         <v>55</v>
@@ -1771,7 +1789,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="22"/>
       <c r="B58" s="2" t="s">
         <v>56</v>
@@ -1780,7 +1798,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="22"/>
       <c r="B59" s="9" t="s">
         <v>57</v>
@@ -1801,7 +1819,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="22"/>
       <c r="B60" s="9" t="s">
         <v>58</v>
@@ -1819,7 +1837,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="22"/>
       <c r="B61" s="10" t="s">
         <v>59</v>
@@ -1840,7 +1858,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="22"/>
       <c r="B62" s="9" t="s">
         <v>60</v>
@@ -1861,7 +1879,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="22"/>
       <c r="B63" s="2" t="s">
         <v>61</v>
@@ -1870,7 +1888,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="22"/>
       <c r="B64" s="2" t="s">
         <v>62</v>
@@ -1879,7 +1897,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="22"/>
       <c r="B65" s="9" t="s">
         <v>63</v>
@@ -1900,7 +1918,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="22"/>
       <c r="B66" s="2" t="s">
         <v>64</v>
@@ -1909,7 +1927,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="22"/>
       <c r="B67" t="s">
         <v>65</v>
@@ -1918,7 +1936,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="22"/>
       <c r="B68" s="9" t="s">
         <v>66</v>
@@ -1939,7 +1957,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="22"/>
       <c r="B69" t="s">
         <v>67</v>
@@ -1948,7 +1966,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="22"/>
       <c r="B70" s="2" t="s">
         <v>68</v>
@@ -1957,7 +1975,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" s="22"/>
       <c r="B71" t="s">
         <v>69</v>
@@ -1966,7 +1984,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" s="22"/>
       <c r="B72" s="17" t="s">
         <v>70</v>
@@ -1975,71 +1993,71 @@
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B80" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="2:2">
+    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B81" s="2"/>
     </row>
-    <row r="82" spans="2:2">
+    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B82" s="2"/>
     </row>
-    <row r="83" spans="2:2">
+    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B83" s="2"/>
     </row>
-    <row r="84" spans="2:2">
+    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B84" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="85" spans="2:2">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B85" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="2:2">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B86" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="87" spans="2:2">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B87" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="2:2">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B88" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="2:2">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B89" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="90" spans="2:2">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B90" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="91" spans="2:2">
+    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B91" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="92" spans="2:2">
+    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B92" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="93" spans="2:2">
+    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B93" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="94" spans="2:2">
+    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B94" s="2" t="s">
         <v>75</v>
       </c>
@@ -2090,9 +2108,11 @@
     <hyperlink ref="F15" r:id="rId39" xr:uid="{FFF7918C-C271-4715-8A9E-33714A21A205}"/>
     <hyperlink ref="G16" r:id="rId40" xr:uid="{9EF2E5E4-26B3-4594-BB2E-BBAA5C4C11DB}"/>
     <hyperlink ref="F16" r:id="rId41" xr:uid="{0DE4CF76-CC43-4FEB-B7C5-C32B4DA42AC2}"/>
+    <hyperlink ref="G19" r:id="rId42" xr:uid="{5560096C-B19D-4490-8636-F40DC42160DC}"/>
+    <hyperlink ref="F19" r:id="rId43" xr:uid="{9165BC5F-C22E-4B03-9BF4-BD0C4CB8AFA9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId42"/>
+  <pageSetup orientation="portrait" r:id="rId44"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Introduction to Azure Functions
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1448C624-0138-4FE6-B636-0DCFA4E28685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4962E402-4A78-4912-B0F5-53F3BE64EBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="139">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -447,6 +447,12 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Review%20the%20principles%20of%20code%20debugging%20and%20exception%20handling</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/CWT2KDY9?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Choose%20a%20data%20storage%20approach%20in%20Azure</t>
   </si>
 </sst>
 </file>
@@ -1028,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1407,11 +1413,23 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="22"/>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="16" t="s">
-        <v>127</v>
+      <c r="C21" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="5">
+        <v>45339</v>
+      </c>
+      <c r="E21" s="5">
+        <v>45339</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -2110,9 +2128,11 @@
     <hyperlink ref="F16" r:id="rId41" xr:uid="{0DE4CF76-CC43-4FEB-B7C5-C32B4DA42AC2}"/>
     <hyperlink ref="G19" r:id="rId42" xr:uid="{5560096C-B19D-4490-8636-F40DC42160DC}"/>
     <hyperlink ref="F19" r:id="rId43" xr:uid="{9165BC5F-C22E-4B03-9BF4-BD0C4CB8AFA9}"/>
+    <hyperlink ref="F21" r:id="rId44" xr:uid="{F9C11EFE-900A-4464-84B5-24776CD6DC0A}"/>
+    <hyperlink ref="G21" r:id="rId45" xr:uid="{08DCAD8B-4BB2-4F56-B2A7-2D466E30A262}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId44"/>
+  <pageSetup orientation="portrait" r:id="rId46"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Create serverless logic with Azure Functions
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4962E402-4A78-4912-B0F5-53F3BE64EBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9AD90F-2415-4A15-80F4-44CC209CD1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="141">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -453,6 +453,12 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Choose%20a%20data%20storage%20approach%20in%20Azure</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/9NSVJGQU?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Introduction%20to%20Azure%20Functions</t>
   </si>
 </sst>
 </file>
@@ -1034,8 +1040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="78" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="G35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1573,7 +1579,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="22"/>
       <c r="B33" s="2" t="s">
         <v>31</v>
@@ -1582,7 +1588,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="22"/>
       <c r="B34" s="2" t="s">
         <v>32</v>
@@ -1591,7 +1597,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="22"/>
       <c r="B35" s="2" t="s">
         <v>33</v>
@@ -1600,7 +1606,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="22"/>
       <c r="B36" s="11" t="s">
         <v>34</v>
@@ -1618,7 +1624,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="22"/>
       <c r="B37" s="2" t="s">
         <v>35</v>
@@ -1627,7 +1633,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="22"/>
       <c r="B38" s="2" t="s">
         <v>36</v>
@@ -1636,7 +1642,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="22"/>
       <c r="B39" s="2" t="s">
         <v>37</v>
@@ -1645,7 +1651,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="22"/>
       <c r="B40" s="2" t="s">
         <v>38</v>
@@ -1654,16 +1660,28 @@
         <v>127</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="22"/>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C41" s="16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C41" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="5">
+        <v>45339</v>
+      </c>
+      <c r="E41" s="5">
+        <v>45339</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="22"/>
       <c r="B42" s="2" t="s">
         <v>40</v>
@@ -1672,7 +1690,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="22"/>
       <c r="B43" s="2" t="s">
         <v>41</v>
@@ -1681,7 +1699,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="22"/>
       <c r="B44" s="2" t="s">
         <v>42</v>
@@ -1690,7 +1708,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="22"/>
       <c r="B45" s="2" t="s">
         <v>43</v>
@@ -1699,7 +1717,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="22"/>
       <c r="B46" s="2" t="s">
         <v>44</v>
@@ -1708,7 +1726,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="22"/>
       <c r="B47" s="2" t="s">
         <v>45</v>
@@ -1717,7 +1735,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="22"/>
       <c r="B48" s="2" t="s">
         <v>46</v>
@@ -2130,9 +2148,11 @@
     <hyperlink ref="F19" r:id="rId43" xr:uid="{9165BC5F-C22E-4B03-9BF4-BD0C4CB8AFA9}"/>
     <hyperlink ref="F21" r:id="rId44" xr:uid="{F9C11EFE-900A-4464-84B5-24776CD6DC0A}"/>
     <hyperlink ref="G21" r:id="rId45" xr:uid="{08DCAD8B-4BB2-4F56-B2A7-2D466E30A262}"/>
+    <hyperlink ref="F41" r:id="rId46" xr:uid="{F59C6ECD-3640-4375-AD4E-7E727F633786}"/>
+    <hyperlink ref="G41" r:id="rId47" xr:uid="{DFA030C7-4148-461A-A6F1-0298DBBEEF1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId46"/>
+  <pageSetup orientation="portrait" r:id="rId48"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Publish a web app to Azure with Visual Studio
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9AD90F-2415-4A15-80F4-44CC209CD1DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7000C818-6755-4F18-9D80-BBB38B41AB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="143">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -459,6 +459,12 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Introduction%20to%20Azure%20Functions</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/ZPFLRBE2?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Create%20serverless%20logic%20with%20Azure%20Functions</t>
   </si>
 </sst>
 </file>
@@ -1040,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" topLeftCell="G18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1581,11 +1587,23 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="22"/>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="16" t="s">
-        <v>127</v>
+      <c r="C33" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D33" s="5">
+        <v>45339</v>
+      </c>
+      <c r="E33" s="5">
+        <v>45339</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
@@ -2150,9 +2168,11 @@
     <hyperlink ref="G21" r:id="rId45" xr:uid="{08DCAD8B-4BB2-4F56-B2A7-2D466E30A262}"/>
     <hyperlink ref="F41" r:id="rId46" xr:uid="{F59C6ECD-3640-4375-AD4E-7E727F633786}"/>
     <hyperlink ref="G41" r:id="rId47" xr:uid="{DFA030C7-4148-461A-A6F1-0298DBBEEF1A}"/>
+    <hyperlink ref="F33" r:id="rId48" xr:uid="{4899D204-6FD8-49A2-ACD8-13E25F5A020A}"/>
+    <hyperlink ref="G33" r:id="rId49" xr:uid="{EF79B9F5-A239-4B5C-B681-566319C8F7B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId48"/>
+  <pageSetup orientation="portrait" r:id="rId50"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Classify images with Azure AI Custom
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7000C818-6755-4F18-9D80-BBB38B41AB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D333BB-65B5-4FDB-966D-E8490CD4E900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="145">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -326,9 +326,6 @@
     <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma-0254/PT7ZCPU4?sharingId=7BBBB75FB7AF740D</t>
   </si>
   <si>
-    <t>https://learn.microsoft.com/en-us/users/shubhamverma-0254/</t>
-  </si>
-  <si>
     <t>Shubham Verma(Shubham.Verma@atqor.com)</t>
   </si>
   <si>
@@ -465,6 +462,15 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Create%20serverless%20logic%20with%20Azure%20Functions</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/9NSMR9HU?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/en-us/users/shubhamverma/</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Publish%20a%20web%20app%20to%20Azure%20with%20Visual%20Studio</t>
   </si>
 </sst>
 </file>
@@ -705,10 +711,10 @@
     <xf numFmtId="0" fontId="6" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1046,8 +1052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1062,10 +1068,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>96</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="24.6" customHeight="1" x14ac:dyDescent="0.4">
@@ -1092,7 +1098,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>74</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1115,7 +1121,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="22"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
@@ -1129,11 +1135,11 @@
         <v>45338</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="22"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
@@ -1147,20 +1153,20 @@
         <v>45338</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="22"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="22"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="12" t="s">
         <v>5</v>
       </c>
@@ -1174,11 +1180,11 @@
         <v>45338</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="22"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
@@ -1192,14 +1198,14 @@
         <v>45237</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="22"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="11" t="s">
         <v>7</v>
       </c>
@@ -1213,11 +1219,11 @@
         <v>45334</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="22"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="11" t="s">
         <v>8</v>
       </c>
@@ -1231,11 +1237,11 @@
         <v>45338</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="22"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="11" t="s">
         <v>9</v>
       </c>
@@ -1249,11 +1255,11 @@
         <v>45337</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="22"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="11" t="s">
         <v>10</v>
       </c>
@@ -1267,11 +1273,11 @@
         <v>45338</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="22"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="11" t="s">
         <v>11</v>
       </c>
@@ -1285,20 +1291,20 @@
         <v>45338</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="22"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="17" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="22"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="9" t="s">
         <v>13</v>
       </c>
@@ -1312,15 +1318,15 @@
         <v>45339</v>
       </c>
       <c r="F15" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G15" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>132</v>
-      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="22"/>
-      <c r="B16" s="23" t="s">
+      <c r="A16" s="23"/>
+      <c r="B16" s="22" t="s">
         <v>14</v>
       </c>
       <c r="C16" s="15" t="s">
@@ -1333,14 +1339,14 @@
         <v>45339</v>
       </c>
       <c r="F16" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>134</v>
-      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="22"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="9" t="s">
         <v>15</v>
       </c>
@@ -1354,14 +1360,14 @@
         <v>45335</v>
       </c>
       <c r="F17" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>99</v>
-      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="22"/>
+      <c r="A18" s="23"/>
       <c r="B18" s="9" t="s">
         <v>16</v>
       </c>
@@ -1382,7 +1388,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="22"/>
+      <c r="A19" s="23"/>
       <c r="B19" s="9" t="s">
         <v>17</v>
       </c>
@@ -1396,14 +1402,14 @@
         <v>45339</v>
       </c>
       <c r="F19" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>136</v>
-      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="22"/>
+      <c r="A20" s="23"/>
       <c r="B20" s="9" t="s">
         <v>18</v>
       </c>
@@ -1417,14 +1423,14 @@
         <v>45337</v>
       </c>
       <c r="F20" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G20" s="6" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="22"/>
+      <c r="A21" s="23"/>
       <c r="B21" s="9" t="s">
         <v>19</v>
       </c>
@@ -1438,50 +1444,62 @@
         <v>45339</v>
       </c>
       <c r="F21" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G21" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="22"/>
-      <c r="B22" s="2" t="s">
+      <c r="A22" s="23"/>
+      <c r="B22" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="16" t="s">
-        <v>127</v>
+      <c r="C22" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="5">
+        <v>45339</v>
+      </c>
+      <c r="E22" s="5">
+        <v>45339</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="22"/>
+      <c r="A23" s="23"/>
       <c r="B23" s="2" t="s">
         <v>21</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="22"/>
+      <c r="A24" s="23"/>
       <c r="B24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C24" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="22"/>
+      <c r="A25" s="23"/>
       <c r="B25" s="2" t="s">
         <v>23</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="22"/>
+      <c r="A26" s="23"/>
       <c r="B26" s="11" t="s">
         <v>24</v>
       </c>
@@ -1495,20 +1513,20 @@
         <v>45339</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="22"/>
+      <c r="A27" s="23"/>
       <c r="B27" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="22"/>
+      <c r="A28" s="23"/>
       <c r="B28" s="9" t="s">
         <v>26</v>
       </c>
@@ -1525,11 +1543,11 @@
         <v>90</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="22"/>
+      <c r="A29" s="23"/>
       <c r="B29" s="9" t="s">
         <v>27</v>
       </c>
@@ -1543,23 +1561,23 @@
         <v>45337</v>
       </c>
       <c r="F29" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="G29" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="G29" s="6" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="22"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="2" t="s">
         <v>28</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="22"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="9" t="s">
         <v>29</v>
       </c>
@@ -1573,20 +1591,20 @@
         <v>45337</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="22"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="22"/>
+      <c r="A33" s="23"/>
       <c r="B33" s="9" t="s">
         <v>31</v>
       </c>
@@ -1600,32 +1618,32 @@
         <v>45339</v>
       </c>
       <c r="F33" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="G33" s="6" t="s">
-        <v>142</v>
-      </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="22"/>
+      <c r="A34" s="23"/>
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="22"/>
+      <c r="A35" s="23"/>
       <c r="B35" s="2" t="s">
         <v>33</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="22"/>
+      <c r="A36" s="23"/>
       <c r="B36" s="11" t="s">
         <v>34</v>
       </c>
@@ -1639,47 +1657,47 @@
         <v>45337</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="22"/>
+      <c r="A37" s="23"/>
       <c r="B37" s="2" t="s">
         <v>35</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="22"/>
+      <c r="A38" s="23"/>
       <c r="B38" s="2" t="s">
         <v>36</v>
       </c>
       <c r="C38" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="22"/>
+      <c r="A39" s="23"/>
       <c r="B39" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="22"/>
+      <c r="A40" s="23"/>
       <c r="B40" s="2" t="s">
         <v>38</v>
       </c>
       <c r="C40" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="22"/>
+      <c r="A41" s="23"/>
       <c r="B41" s="9" t="s">
         <v>39</v>
       </c>
@@ -1693,167 +1711,167 @@
         <v>45339</v>
       </c>
       <c r="F41" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="G41" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="G41" s="6" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="22"/>
+      <c r="A42" s="23"/>
       <c r="B42" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="22"/>
+      <c r="A43" s="23"/>
       <c r="B43" s="2" t="s">
         <v>41</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="22"/>
+      <c r="A44" s="23"/>
       <c r="B44" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="22"/>
+      <c r="A45" s="23"/>
       <c r="B45" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="22"/>
+      <c r="A46" s="23"/>
       <c r="B46" s="2" t="s">
         <v>44</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="22"/>
+      <c r="A47" s="23"/>
       <c r="B47" s="2" t="s">
         <v>45</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="22"/>
+      <c r="A48" s="23"/>
       <c r="B48" s="2" t="s">
         <v>46</v>
       </c>
       <c r="C48" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="22"/>
+      <c r="A49" s="23"/>
       <c r="B49" s="2" t="s">
         <v>47</v>
       </c>
       <c r="C49" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="22"/>
+      <c r="A50" s="23"/>
       <c r="B50" s="21" t="s">
         <v>48</v>
       </c>
       <c r="C50" s="20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="22"/>
+      <c r="A51" s="23"/>
       <c r="B51" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C51" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="22"/>
+      <c r="A52" s="23"/>
       <c r="B52" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C52" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="22"/>
+      <c r="A53" s="23"/>
       <c r="B53" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C53" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="22"/>
+      <c r="A54" s="23"/>
       <c r="B54" s="2" t="s">
         <v>52</v>
       </c>
       <c r="C54" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="22"/>
+      <c r="A55" s="23"/>
       <c r="B55" s="2" t="s">
         <v>53</v>
       </c>
       <c r="C55" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="22"/>
+      <c r="A56" s="23"/>
       <c r="B56" s="2" t="s">
         <v>54</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="22"/>
+      <c r="A57" s="23"/>
       <c r="B57" s="2" t="s">
         <v>55</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="22"/>
+      <c r="A58" s="23"/>
       <c r="B58" s="2" t="s">
         <v>56</v>
       </c>
       <c r="C58" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="22"/>
+      <c r="A59" s="23"/>
       <c r="B59" s="9" t="s">
         <v>57</v>
       </c>
@@ -1867,14 +1885,14 @@
         <v>45336</v>
       </c>
       <c r="F59" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="22"/>
+      <c r="A60" s="23"/>
       <c r="B60" s="9" t="s">
         <v>58</v>
       </c>
@@ -1888,11 +1906,11 @@
         <v>45337</v>
       </c>
       <c r="F60" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="22"/>
+      <c r="A61" s="23"/>
       <c r="B61" s="10" t="s">
         <v>59</v>
       </c>
@@ -1906,14 +1924,14 @@
         <v>45336</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="22"/>
+      <c r="A62" s="23"/>
       <c r="B62" s="9" t="s">
         <v>60</v>
       </c>
@@ -1927,32 +1945,32 @@
         <v>45337</v>
       </c>
       <c r="F62" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G62" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="G62" s="6" t="s">
-        <v>108</v>
-      </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="22"/>
+      <c r="A63" s="23"/>
       <c r="B63" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A64" s="22"/>
+      <c r="A64" s="23"/>
       <c r="B64" s="2" t="s">
         <v>62</v>
       </c>
       <c r="C64" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A65" s="22"/>
+      <c r="A65" s="23"/>
       <c r="B65" s="9" t="s">
         <v>63</v>
       </c>
@@ -1966,32 +1984,32 @@
         <v>45337</v>
       </c>
       <c r="F65" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="G65" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="G65" s="6" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A66" s="22"/>
+      <c r="A66" s="23"/>
       <c r="B66" s="2" t="s">
         <v>64</v>
       </c>
       <c r="C66" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A67" s="22"/>
+      <c r="A67" s="23"/>
       <c r="B67" t="s">
         <v>65</v>
       </c>
       <c r="C67" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A68" s="22"/>
+      <c r="A68" s="23"/>
       <c r="B68" s="9" t="s">
         <v>66</v>
       </c>
@@ -2005,46 +2023,46 @@
         <v>45336</v>
       </c>
       <c r="F68" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G68" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="G68" s="6" t="s">
-        <v>106</v>
-      </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A69" s="22"/>
+      <c r="A69" s="23"/>
       <c r="B69" t="s">
         <v>67</v>
       </c>
       <c r="C69" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A70" s="22"/>
+      <c r="A70" s="23"/>
       <c r="B70" s="2" t="s">
         <v>68</v>
       </c>
       <c r="C70" s="16" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A71" s="22"/>
+      <c r="A71" s="23"/>
       <c r="B71" t="s">
         <v>69</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A72" s="22"/>
+      <c r="A72" s="23"/>
       <c r="B72" s="17" t="s">
         <v>70</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.3">
@@ -2170,27 +2188,29 @@
     <hyperlink ref="G41" r:id="rId47" xr:uid="{DFA030C7-4148-461A-A6F1-0298DBBEEF1A}"/>
     <hyperlink ref="F33" r:id="rId48" xr:uid="{4899D204-6FD8-49A2-ACD8-13E25F5A020A}"/>
     <hyperlink ref="G33" r:id="rId49" xr:uid="{EF79B9F5-A239-4B5C-B681-566319C8F7B2}"/>
+    <hyperlink ref="F22" r:id="rId50" xr:uid="{29FC98B9-D1A5-4DA3-BEB0-A66992D3665E}"/>
+    <hyperlink ref="G22" r:id="rId51" xr:uid="{6F5CAB67-6F2F-4B45-A639-8263585BF2F8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId50"/>
+  <pageSetup orientation="portrait" r:id="rId52"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1f23d82e-0582-47b0-ad17-93a33fa50ca6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1f23d82e-0582-47b0-ad17-93a33fa50ca6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2415,6 +2435,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D7E8C91-0848-41CA-95C1-FE9D8052D59D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99BD043-E710-4524-8574-E9A47DF2271E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2427,14 +2455,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="1f23d82e-0582-47b0-ad17-93a33fa50ca6"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D7E8C91-0848-41CA-95C1-FE9D8052D59D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Introduction to Web Development with Blazor
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D333BB-65B5-4FDB-966D-E8490CD4E900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA8C0FA-C295-4259-B11E-39475FEB4B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="147">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -471,6 +471,12 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Publish%20a%20web%20app%20to%20Azure%20with%20Visual%20Studio</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/24XCJ9JV?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Classify%20images%20with%20Azure%20AI%20Custom</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1059,7 @@
   <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1473,11 +1479,23 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="23"/>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="16" t="s">
-        <v>126</v>
+      <c r="C23" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="5">
+        <v>45340</v>
+      </c>
+      <c r="E23" s="5">
+        <v>45340</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -2190,9 +2208,11 @@
     <hyperlink ref="G33" r:id="rId49" xr:uid="{EF79B9F5-A239-4B5C-B681-566319C8F7B2}"/>
     <hyperlink ref="F22" r:id="rId50" xr:uid="{29FC98B9-D1A5-4DA3-BEB0-A66992D3665E}"/>
     <hyperlink ref="G22" r:id="rId51" xr:uid="{6F5CAB67-6F2F-4B45-A639-8263585BF2F8}"/>
+    <hyperlink ref="F23" r:id="rId52" xr:uid="{A80C9A86-9B04-48A1-9074-01BB9DEC8B98}"/>
+    <hyperlink ref="G23" r:id="rId53" xr:uid="{05DC9EF2-7114-47C0-BF81-4A215354682C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId52"/>
+  <pageSetup orientation="portrait" r:id="rId54"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Store applicationStore application data with Azure Blob Storage data with Azure Blob Storage
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA8C0FA-C295-4259-B11E-39475FEB4B7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA9C37D-9C95-42F1-BB2F-667BAC96E895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="149">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -477,6 +477,12 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Classify%20images%20with%20Azure%20AI%20Custom</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/WACBMH5N?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Introduction%20to%20Web%20Development%20with%20Blazor</t>
   </si>
 </sst>
 </file>
@@ -1059,7 +1065,7 @@
   <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1500,11 +1506,23 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="16" t="s">
-        <v>126</v>
+      <c r="C24" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="5">
+        <v>45340</v>
+      </c>
+      <c r="E24" s="5">
+        <v>45340</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -2210,9 +2228,11 @@
     <hyperlink ref="G22" r:id="rId51" xr:uid="{6F5CAB67-6F2F-4B45-A639-8263585BF2F8}"/>
     <hyperlink ref="F23" r:id="rId52" xr:uid="{A80C9A86-9B04-48A1-9074-01BB9DEC8B98}"/>
     <hyperlink ref="G23" r:id="rId53" xr:uid="{05DC9EF2-7114-47C0-BF81-4A215354682C}"/>
+    <hyperlink ref="F24" r:id="rId54" xr:uid="{1E8EE262-AD22-4353-98CE-1E036CB9D156}"/>
+    <hyperlink ref="G24" r:id="rId55" xr:uid="{F8007B43-EC43-44E9-8B81-542BF6AE9867}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId54"/>
+  <pageSetup orientation="portrait" r:id="rId56"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Translate text and speech with Azure AI services
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA9C37D-9C95-42F1-BB2F-667BAC96E895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF318B3-D121-4708-B9FD-21E8366A3ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="151">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -483,6 +483,12 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Introduction%20to%20Web%20Development%20with%20Blazor</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/FZUJBPQX?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Store%20application%20data%20with%20Azure%20Blob%20Storage</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1071,7 @@
   <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1527,11 +1533,23 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="23"/>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="16" t="s">
-        <v>126</v>
+      <c r="C25" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="5">
+        <v>45340</v>
+      </c>
+      <c r="E25" s="5">
+        <v>45340</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -2230,27 +2248,29 @@
     <hyperlink ref="G23" r:id="rId53" xr:uid="{05DC9EF2-7114-47C0-BF81-4A215354682C}"/>
     <hyperlink ref="F24" r:id="rId54" xr:uid="{1E8EE262-AD22-4353-98CE-1E036CB9D156}"/>
     <hyperlink ref="G24" r:id="rId55" xr:uid="{F8007B43-EC43-44E9-8B81-542BF6AE9867}"/>
+    <hyperlink ref="F25" r:id="rId56" xr:uid="{F870A5ED-1040-413C-9957-8AB4DA54F1AE}"/>
+    <hyperlink ref="G25" r:id="rId57" xr:uid="{9305D30B-F588-45C8-B5FB-44338C11D842}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId56"/>
+  <pageSetup orientation="portrait" r:id="rId58"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1f23d82e-0582-47b0-ad17-93a33fa50ca6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1f23d82e-0582-47b0-ad17-93a33fa50ca6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2475,14 +2495,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D7E8C91-0848-41CA-95C1-FE9D8052D59D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99BD043-E710-4524-8574-E9A47DF2271E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2495,6 +2507,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="1f23d82e-0582-47b0-ad17-93a33fa50ca6"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D7E8C91-0848-41CA-95C1-FE9D8052D59D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Scale an App Service web app to efficiently meet demand with App Service scale up and scale out
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF318B3-D121-4708-B9FD-21E8366A3ACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD7990A-6B87-44CF-B4FC-6059A11B4807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="153">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -489,6 +489,12 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Store%20application%20data%20with%20Azure%20Blob%20Storage</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/9NSEQ4EU?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Translate%20text%20and%20speech%20with%20Azure%20AI%20services</t>
   </si>
 </sst>
 </file>
@@ -1070,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1572,11 +1578,23 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="23"/>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="16" t="s">
-        <v>126</v>
+      <c r="C27" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D27" s="5">
+        <v>45340</v>
+      </c>
+      <c r="E27" s="5">
+        <v>45340</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -2250,27 +2268,29 @@
     <hyperlink ref="G24" r:id="rId55" xr:uid="{F8007B43-EC43-44E9-8B81-542BF6AE9867}"/>
     <hyperlink ref="F25" r:id="rId56" xr:uid="{F870A5ED-1040-413C-9957-8AB4DA54F1AE}"/>
     <hyperlink ref="G25" r:id="rId57" xr:uid="{9305D30B-F588-45C8-B5FB-44338C11D842}"/>
+    <hyperlink ref="F27" r:id="rId58" xr:uid="{97F75583-0939-4B97-8496-1097C4E65793}"/>
+    <hyperlink ref="G27" r:id="rId59" xr:uid="{A82F71AF-6C15-4271-BE43-692C913FE62D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId58"/>
+  <pageSetup orientation="portrait" r:id="rId60"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1f23d82e-0582-47b0-ad17-93a33fa50ca6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1f23d82e-0582-47b0-ad17-93a33fa50ca6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2495,6 +2515,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D7E8C91-0848-41CA-95C1-FE9D8052D59D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99BD043-E710-4524-8574-E9A47DF2271E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2507,14 +2535,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="1f23d82e-0582-47b0-ad17-93a33fa50ca6"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D7E8C91-0848-41CA-95C1-FE9D8052D59D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Stage a web app deployment for testing and rollback by using App Service deployment slot
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD7990A-6B87-44CF-B4FC-6059A11B4807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7168C2-4512-4BEC-BA69-75947EDC482D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="155">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -495,6 +495,12 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Translate%20text%20and%20speech%20with%20Azure%20AI%20services</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/8R6DFKMW?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Scale%20an%20App%20Service%20web%20app%20to%20efficiently%20meet%20demand%20with%20App%20Service%20scale%20up%20and%20scale%20out</t>
   </si>
 </sst>
 </file>
@@ -1076,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="81" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,7 +1093,7 @@
     <col min="3" max="4" width="18.109375" customWidth="1"/>
     <col min="5" max="5" width="21.21875" customWidth="1"/>
     <col min="6" max="6" width="122.6640625" customWidth="1"/>
-    <col min="7" max="7" width="152.77734375" customWidth="1"/>
+    <col min="7" max="7" width="190.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1641,11 +1647,23 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="23"/>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="16" t="s">
-        <v>126</v>
+      <c r="C30" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" s="5">
+        <v>45340</v>
+      </c>
+      <c r="E30" s="5">
+        <v>45340</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -2270,27 +2288,29 @@
     <hyperlink ref="G25" r:id="rId57" xr:uid="{9305D30B-F588-45C8-B5FB-44338C11D842}"/>
     <hyperlink ref="F27" r:id="rId58" xr:uid="{97F75583-0939-4B97-8496-1097C4E65793}"/>
     <hyperlink ref="G27" r:id="rId59" xr:uid="{A82F71AF-6C15-4271-BE43-692C913FE62D}"/>
+    <hyperlink ref="F30" r:id="rId60" xr:uid="{63AD2017-9B8B-46D4-951B-B8B1A1EF1988}"/>
+    <hyperlink ref="G30" r:id="rId61" xr:uid="{8ADB8D3B-EAE7-46A1-944B-49287511FC8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId60"/>
+  <pageSetup orientation="portrait" r:id="rId62"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1f23d82e-0582-47b0-ad17-93a33fa50ca6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1f23d82e-0582-47b0-ad17-93a33fa50ca6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2515,14 +2535,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D7E8C91-0848-41CA-95C1-FE9D8052D59D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99BD043-E710-4524-8574-E9A47DF2271E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2535,6 +2547,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="1f23d82e-0582-47b0-ad17-93a33fa50ca6"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D7E8C91-0848-41CA-95C1-FE9D8052D59D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Chain Azure Functions together using input and output bindings
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF7168C2-4512-4BEC-BA69-75947EDC482D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398C09B7-6AFC-4D7A-9A9D-A4238739303F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="159">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -501,6 +501,18 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Scale%20an%20App%20Service%20web%20app%20to%20efficiently%20meet%20demand%20with%20App%20Service%20scale%20up%20and%20scale%20out</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Stage%20a%20web%20app%20deployment%20for%20testing%20and%20rollback%20by%20using%20App%20Service%20deployment%20slot</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/AQW9HSD7?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/PTZYCFM4?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Expose%20multiple%20Azure%20Function%20apps%20as%20a%20consistent%20API%20by%20using%20Azure%20API%20Management</t>
   </si>
 </sst>
 </file>
@@ -1082,8 +1094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="81" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="93" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1686,11 +1698,23 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="23"/>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="16" t="s">
-        <v>126</v>
+      <c r="C32" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D32" s="5">
+        <v>45341</v>
+      </c>
+      <c r="E32" s="5">
+        <v>45341</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -1716,11 +1740,23 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="23"/>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="16" t="s">
-        <v>126</v>
+      <c r="C34" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="5">
+        <v>45341</v>
+      </c>
+      <c r="E34" s="5">
+        <v>45341</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
@@ -2290,9 +2326,13 @@
     <hyperlink ref="G27" r:id="rId59" xr:uid="{A82F71AF-6C15-4271-BE43-692C913FE62D}"/>
     <hyperlink ref="F30" r:id="rId60" xr:uid="{63AD2017-9B8B-46D4-951B-B8B1A1EF1988}"/>
     <hyperlink ref="G30" r:id="rId61" xr:uid="{8ADB8D3B-EAE7-46A1-944B-49287511FC8C}"/>
+    <hyperlink ref="G32" r:id="rId62" xr:uid="{DE80A3DF-C3A2-4386-95F8-3C22A7E1279B}"/>
+    <hyperlink ref="F32" r:id="rId63" xr:uid="{E495ADB0-B13C-4B40-B8D9-CDAD519770FF}"/>
+    <hyperlink ref="F34" r:id="rId64" xr:uid="{278D4DC0-9FB2-458B-B620-BCE7AE486CB7}"/>
+    <hyperlink ref="G34" r:id="rId65" xr:uid="{E4D8B555-DB5F-4A28-8BB0-561E27D76B61}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId62"/>
+  <pageSetup orientation="portrait" r:id="rId66"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Develop, test, and deploy an Azure Function with Visual Studio
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398C09B7-6AFC-4D7A-9A9D-A4238739303F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374EF798-1C8F-4DE2-BA6D-88DA56B3C205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="164">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -513,6 +513,21 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Expose%20multiple%20Azure%20Function%20apps%20as%20a%20consistent%20API%20by%20using%20Azure%20API%20Management</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/N79LKD3F?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Chain%20Azure%20Functions%20together%20using%20input%20and%20output%20bindings</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Write%20your%20first%20PowerShell%20code</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/AQWUUUU7?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Execute%20an%20Azure%20Function%20with%20triggers</t>
   </si>
 </sst>
 </file>
@@ -1094,8 +1109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="93" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E47" sqref="E47"/>
+    <sheetView tabSelected="1" topLeftCell="G31" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1761,11 +1776,23 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="23"/>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="16" t="s">
-        <v>126</v>
+      <c r="C35" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="5">
+        <v>45341</v>
+      </c>
+      <c r="E35" s="5">
+        <v>45341</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
@@ -1785,14 +1812,29 @@
       <c r="F36" s="6" t="s">
         <v>119</v>
       </c>
+      <c r="G36" s="6" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="23"/>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="16" t="s">
-        <v>126</v>
+      <c r="C37" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D37" s="5">
+        <v>45341</v>
+      </c>
+      <c r="E37" s="5">
+        <v>45341</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
@@ -2330,9 +2372,14 @@
     <hyperlink ref="F32" r:id="rId63" xr:uid="{E495ADB0-B13C-4B40-B8D9-CDAD519770FF}"/>
     <hyperlink ref="F34" r:id="rId64" xr:uid="{278D4DC0-9FB2-458B-B620-BCE7AE486CB7}"/>
     <hyperlink ref="G34" r:id="rId65" xr:uid="{E4D8B555-DB5F-4A28-8BB0-561E27D76B61}"/>
+    <hyperlink ref="F35" r:id="rId66" xr:uid="{ACCA7EE8-03DC-44A0-9201-C1B9C03D57C0}"/>
+    <hyperlink ref="G35" r:id="rId67" xr:uid="{8FAB8F60-8419-455B-A675-AD0DDA52B488}"/>
+    <hyperlink ref="G36" r:id="rId68" xr:uid="{3EDC3B5B-4CBB-4840-B603-4BE0BA431721}"/>
+    <hyperlink ref="F37" r:id="rId69" xr:uid="{BFB42495-16A9-4D49-BF06-A4B57961115C}"/>
+    <hyperlink ref="G37" r:id="rId70" xr:uid="{F8251AEF-CB35-45F4-86D7-7B0E42F9C7DE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId66"/>
+  <pageSetup orientation="portrait" r:id="rId71"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Develop, test, and publish Azure Functions by using Azure Functions Core Tools
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{374EF798-1C8F-4DE2-BA6D-88DA56B3C205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C9BA56-CFCD-4B3B-A6E7-8EC95D231D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="166">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -528,6 +528,12 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Execute%20an%20Azure%20Function%20with%20triggers</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/BLMWQMAD?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Develop%2C%20test%2C%20and%20deploy%20an%20Azure%20Function%20with%20Visual%20Studio</t>
   </si>
 </sst>
 </file>
@@ -1109,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G31" zoomScale="125" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G35" zoomScale="115" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
@@ -1839,11 +1845,23 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="23"/>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="16" t="s">
-        <v>126</v>
+      <c r="C38" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="5">
+        <v>45339</v>
+      </c>
+      <c r="E38" s="5">
+        <v>45339</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
@@ -2377,9 +2395,11 @@
     <hyperlink ref="G36" r:id="rId68" xr:uid="{3EDC3B5B-4CBB-4840-B603-4BE0BA431721}"/>
     <hyperlink ref="F37" r:id="rId69" xr:uid="{BFB42495-16A9-4D49-BF06-A4B57961115C}"/>
     <hyperlink ref="G37" r:id="rId70" xr:uid="{F8251AEF-CB35-45F4-86D7-7B0E42F9C7DE}"/>
+    <hyperlink ref="F38" r:id="rId71" xr:uid="{69D2BDC0-5A61-4E03-9DF4-475C9F219536}"/>
+    <hyperlink ref="G38" r:id="rId72" xr:uid="{D425346B-BE74-40EA-957C-8086B11202CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId71"/>
+  <pageSetup orientation="portrait" r:id="rId73"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Introduction to Azure Logic Apps
</commit_message>
<xml_diff>
--- a/ShubhamVermaLearningAzureLearningModule.xlsx
+++ b/ShubhamVermaLearningAzureLearningModule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\AzureModule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C9BA56-CFCD-4B3B-A6E7-8EC95D231D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BAD951-DF32-4D81-8AAA-0A606A97155B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="598" xr2:uid="{A84A4CFD-8C9A-4323-8013-324012D78EAC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="171">
   <si>
     <t>Mandatory (Training modules)</t>
   </si>
@@ -534,6 +534,21 @@
   </si>
   <si>
     <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Develop%2C%20test%2C%20and%20deploy%20an%20Azure%20Function%20with%20Visual%20Studio</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/J6E2BQ8T?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://github.com/ShubhamVermaTheDeveloper/AzureModuleLearning/tree/main/Develop%2C%20test%2C%20and%20publish%20Azure%20Functions%20by%20using%20Azure%20Functions%20Core%20Tools</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/N799EGVF?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/9NSSQ7EU?sharingId=7BBBB75FB7AF740D</t>
+  </si>
+  <si>
+    <t>https://learn.microsoft.com/api/achievements/share/en-us/ShubhamVerma/N799JNEF?sharingId=7BBBB75FB7AF740D</t>
   </si>
 </sst>
 </file>
@@ -1115,8 +1130,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03BA2E33-66EB-440B-9957-8C5E18B127A0}">
   <dimension ref="A1:G94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G35" zoomScale="115" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="D37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1866,11 +1881,23 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="23"/>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="16" t="s">
-        <v>126</v>
+      <c r="C39" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="5">
+        <v>45341</v>
+      </c>
+      <c r="E39" s="5">
+        <v>45341</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
@@ -1959,11 +1986,20 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="23"/>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="16" t="s">
-        <v>126</v>
+      <c r="C48" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="5">
+        <v>45342</v>
+      </c>
+      <c r="E48" s="5">
+        <v>45342</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
@@ -1986,11 +2022,20 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="23"/>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C51" s="16" t="s">
-        <v>126</v>
+      <c r="C51" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D51" s="5">
+        <v>45342</v>
+      </c>
+      <c r="E51" s="5">
+        <v>45342</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
@@ -2013,11 +2058,20 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="23"/>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="C54" s="16" t="s">
-        <v>126</v>
+      <c r="C54" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D54" s="5">
+        <v>45342</v>
+      </c>
+      <c r="E54" s="5">
+        <v>45342</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
@@ -2397,27 +2451,32 @@
     <hyperlink ref="G37" r:id="rId70" xr:uid="{F8251AEF-CB35-45F4-86D7-7B0E42F9C7DE}"/>
     <hyperlink ref="F38" r:id="rId71" xr:uid="{69D2BDC0-5A61-4E03-9DF4-475C9F219536}"/>
     <hyperlink ref="G38" r:id="rId72" xr:uid="{D425346B-BE74-40EA-957C-8086B11202CB}"/>
+    <hyperlink ref="F39" r:id="rId73" xr:uid="{7E845288-6007-44D5-AD64-705E23617A09}"/>
+    <hyperlink ref="G39" r:id="rId74" xr:uid="{246B9E8A-1B44-4096-87B3-05B89EDDBFD0}"/>
+    <hyperlink ref="F48" r:id="rId75" xr:uid="{F764CA36-1681-4B84-BD54-7B70A1DC76D2}"/>
+    <hyperlink ref="F54" r:id="rId76" xr:uid="{91ACB72F-ADA7-4770-9B24-5E8BCAEA3BD6}"/>
+    <hyperlink ref="F51" r:id="rId77" xr:uid="{84EC7774-A20F-4C46-99DC-955631DF451C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId73"/>
+  <pageSetup orientation="portrait" r:id="rId78"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1f23d82e-0582-47b0-ad17-93a33fa50ca6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1f23d82e-0582-47b0-ad17-93a33fa50ca6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2642,6 +2701,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D7E8C91-0848-41CA-95C1-FE9D8052D59D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E99BD043-E710-4524-8574-E9A47DF2271E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -2654,14 +2721,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="1f23d82e-0582-47b0-ad17-93a33fa50ca6"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D7E8C91-0848-41CA-95C1-FE9D8052D59D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>